<commit_message>
Updated 2nd year LBTS values
</commit_message>
<xml_diff>
--- a/figures and tables/2022 Tables/TableS_posterior_subsets.xlsx
+++ b/figures and tables/2022 Tables/TableS_posterior_subsets.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joanna\Documents\GitHub\RiverBiomass\figures and tables\2022 Figures and Tables\tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\Users\jblaszczak\Documents\GitHub\RiverBiomass\figures and tables\2022 Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12CC2BA6-8EB1-4B0E-AB4F-4B15E55D6A12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="23260" windowHeight="12580" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="STS Year 1" sheetId="3" r:id="rId1"/>
@@ -124,7 +123,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
@@ -264,7 +263,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -444,12 +443,6 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -611,16 +604,18 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -975,21 +970,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BC6E831-8C2D-4B6A-99E9-08132E881932}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.33203125" customWidth="1"/>
-    <col min="3" max="3" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.36328125" customWidth="1"/>
+    <col min="3" max="3" width="14.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D1" s="5" t="s">
         <v>7</v>
       </c>
@@ -999,7 +994,7 @@
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -1028,14 +1023,14 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="4" t="s">
         <v>28</v>
       </c>
       <c r="D3" s="2">
@@ -1053,18 +1048,18 @@
       <c r="H3" s="3">
         <v>4604.0787281051798</v>
       </c>
-      <c r="I3" s="6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
+      <c r="I3" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="4" t="s">
         <v>29</v>
       </c>
       <c r="D4" s="2">
@@ -1082,18 +1077,18 @@
       <c r="H4" s="3">
         <v>4056.9857106514901</v>
       </c>
-      <c r="I4" s="6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
+      <c r="I4" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="4" t="s">
         <v>30</v>
       </c>
       <c r="D5" s="2">
@@ -1111,18 +1106,18 @@
       <c r="H5" s="3">
         <v>3737.0130184934201</v>
       </c>
-      <c r="I5" s="6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="6" t="s">
+      <c r="I5" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="4" t="s">
         <v>31</v>
       </c>
       <c r="D6" s="2">
@@ -1140,18 +1135,18 @@
       <c r="H6" s="3">
         <v>2391.9327031100302</v>
       </c>
-      <c r="I6" s="6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="6" t="s">
+      <c r="I6" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="4" t="s">
         <v>16</v>
       </c>
       <c r="D7" s="2">
@@ -1169,18 +1164,18 @@
       <c r="H7" s="3">
         <v>947.81191179775499</v>
       </c>
-      <c r="I7" s="6" t="b">
+      <c r="I7" s="4" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="4" t="s">
         <v>28</v>
       </c>
       <c r="D8" s="2">
@@ -1198,18 +1193,18 @@
       <c r="H8" s="3">
         <v>1126.78386312217</v>
       </c>
-      <c r="I8" s="6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="6" t="s">
+      <c r="I8" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="4" t="s">
         <v>29</v>
       </c>
       <c r="D9" s="2">
@@ -1227,18 +1222,18 @@
       <c r="H9" s="3">
         <v>4409.8758126829598</v>
       </c>
-      <c r="I9" s="6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
+      <c r="I9" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A10" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="4" t="s">
         <v>30</v>
       </c>
       <c r="D10" s="2">
@@ -1256,18 +1251,18 @@
       <c r="H10" s="3">
         <v>3089.5836535718399</v>
       </c>
-      <c r="I10" s="6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
+      <c r="I10" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A11" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="4" t="s">
         <v>31</v>
       </c>
       <c r="D11" s="2">
@@ -1285,18 +1280,18 @@
       <c r="H11" s="3">
         <v>1243.5158816865201</v>
       </c>
-      <c r="I11" s="6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="6" t="s">
+      <c r="I11" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A12" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="4" t="s">
         <v>16</v>
       </c>
       <c r="D12" s="2">
@@ -1314,18 +1309,18 @@
       <c r="H12" s="3">
         <v>818.07155239671602</v>
       </c>
-      <c r="I12" s="6" t="b">
+      <c r="I12" s="4" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="6" t="s">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="4" t="s">
         <v>28</v>
       </c>
       <c r="D13" s="2">
@@ -1343,18 +1338,18 @@
       <c r="H13" s="3">
         <v>2446.8342435101499</v>
       </c>
-      <c r="I13" s="6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="6" t="s">
+      <c r="I13" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A14" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="4" t="s">
         <v>29</v>
       </c>
       <c r="D14" s="2">
@@ -1372,18 +1367,18 @@
       <c r="H14" s="3">
         <v>3379.4645302588201</v>
       </c>
-      <c r="I14" s="6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="6" t="s">
+      <c r="I14" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A15" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="4" t="s">
         <v>30</v>
       </c>
       <c r="D15" s="2">
@@ -1401,18 +1396,18 @@
       <c r="H15" s="3">
         <v>2068.3048573062401</v>
       </c>
-      <c r="I15" s="6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="6" t="s">
+      <c r="I15" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A16" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="4" t="s">
         <v>31</v>
       </c>
       <c r="D16" s="2">
@@ -1430,18 +1425,18 @@
       <c r="H16" s="3">
         <v>2134.8500940213999</v>
       </c>
-      <c r="I16" s="6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="6" t="s">
+      <c r="I16" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A17" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="4" t="s">
         <v>16</v>
       </c>
       <c r="D17" s="2">
@@ -1459,18 +1454,18 @@
       <c r="H17" s="3">
         <v>2184.6733579637898</v>
       </c>
-      <c r="I17" s="6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="6" t="s">
+      <c r="I17" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A18" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="4" t="s">
         <v>28</v>
       </c>
       <c r="D18" s="2">
@@ -1488,18 +1483,18 @@
       <c r="H18" s="3">
         <v>2777.5836158884799</v>
       </c>
-      <c r="I18" s="6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="6" t="s">
+      <c r="I18" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A19" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="4" t="s">
         <v>29</v>
       </c>
       <c r="D19" s="2">
@@ -1517,18 +1512,18 @@
       <c r="H19" s="3">
         <v>2400.3737592531802</v>
       </c>
-      <c r="I19" s="6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="6" t="s">
+      <c r="I19" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A20" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="4" t="s">
         <v>30</v>
       </c>
       <c r="D20" s="2">
@@ -1546,18 +1541,18 @@
       <c r="H20" s="3">
         <v>2244.2731449027501</v>
       </c>
-      <c r="I20" s="6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="6" t="s">
+      <c r="I20" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A21" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="C21" s="4" t="s">
         <v>31</v>
       </c>
       <c r="D21" s="2">
@@ -1575,18 +1570,18 @@
       <c r="H21" s="3">
         <v>1550.3607135882601</v>
       </c>
-      <c r="I21" s="6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="6" t="s">
+      <c r="I21" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A22" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="C22" s="4" t="s">
         <v>16</v>
       </c>
       <c r="D22" s="2">
@@ -1604,18 +1599,18 @@
       <c r="H22" s="3">
         <v>615.801852277335</v>
       </c>
-      <c r="I22" s="6" t="b">
+      <c r="I22" s="4" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="6" t="s">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A23" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="B23" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="C23" s="4" t="s">
         <v>28</v>
       </c>
       <c r="D23" s="2">
@@ -1633,18 +1628,18 @@
       <c r="H23" s="3">
         <v>4047.3062894344098</v>
       </c>
-      <c r="I23" s="6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="6" t="s">
+      <c r="I23" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A24" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B24" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="C24" s="4" t="s">
         <v>29</v>
       </c>
       <c r="D24" s="2">
@@ -1662,18 +1657,18 @@
       <c r="H24" s="3">
         <v>3959.84081958466</v>
       </c>
-      <c r="I24" s="6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="6" t="s">
+      <c r="I24" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A25" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B25" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="C25" s="4" t="s">
         <v>30</v>
       </c>
       <c r="D25" s="2">
@@ -1691,18 +1686,18 @@
       <c r="H25" s="3">
         <v>14103.795597664301</v>
       </c>
-      <c r="I25" s="6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" s="6" t="s">
+      <c r="I25" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A26" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="B26" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="C26" s="4" t="s">
         <v>31</v>
       </c>
       <c r="D26" s="2">
@@ -1720,18 +1715,18 @@
       <c r="H26" s="3">
         <v>1690.4684260024601</v>
       </c>
-      <c r="I26" s="6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" s="6" t="s">
+      <c r="I26" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A27" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B27" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="C27" s="4" t="s">
         <v>16</v>
       </c>
       <c r="D27" s="2">
@@ -1749,18 +1744,18 @@
       <c r="H27" s="3">
         <v>1833.98844044528</v>
       </c>
-      <c r="I27" s="6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A28" s="6" t="s">
+      <c r="I27" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A28" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B28" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C28" s="6" t="s">
+      <c r="C28" s="4" t="s">
         <v>28</v>
       </c>
       <c r="D28" s="2">
@@ -1778,18 +1773,18 @@
       <c r="H28" s="3">
         <v>2414.6409718239802</v>
       </c>
-      <c r="I28" s="6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" s="6" t="s">
+      <c r="I28" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A29" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="B29" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C29" s="6" t="s">
+      <c r="C29" s="4" t="s">
         <v>29</v>
       </c>
       <c r="D29" s="2">
@@ -1807,18 +1802,18 @@
       <c r="H29" s="3">
         <v>2808.8373195579202</v>
       </c>
-      <c r="I29" s="6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30" s="6" t="s">
+      <c r="I29" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A30" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="B30" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C30" s="6" t="s">
+      <c r="C30" s="4" t="s">
         <v>30</v>
       </c>
       <c r="D30" s="2">
@@ -1836,18 +1831,18 @@
       <c r="H30" s="3">
         <v>5491.5172555603303</v>
       </c>
-      <c r="I30" s="6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A31" s="6" t="s">
+      <c r="I30" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A31" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="B31" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C31" s="6" t="s">
+      <c r="C31" s="4" t="s">
         <v>31</v>
       </c>
       <c r="D31" s="2">
@@ -1865,18 +1860,18 @@
       <c r="H31" s="3">
         <v>1869.68130006346</v>
       </c>
-      <c r="I31" s="6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" s="6" t="s">
+      <c r="I31" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A32" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B32" s="6" t="s">
+      <c r="B32" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C32" s="6" t="s">
+      <c r="C32" s="4" t="s">
         <v>16</v>
       </c>
       <c r="D32" s="2">
@@ -1894,12 +1889,12 @@
       <c r="H32" s="3">
         <v>1382.46500234925</v>
       </c>
-      <c r="I32" s="6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B38" s="6"/>
+      <c r="I32" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B38" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1910,28 +1905,28 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1C208C8-382C-4089-80C9-81C36BAAD77B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.81640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="7" width="7.6640625" customWidth="1"/>
+    <col min="3" max="3" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="7.6328125" customWidth="1"/>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.21875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.6640625" customWidth="1"/>
+    <col min="9" max="9" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="6"/>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1" s="4"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
       <c r="D1" s="5" t="s">
         <v>27</v>
       </c>
@@ -1941,43 +1936,43 @@
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="H2" s="6" t="s">
+      <c r="G2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="4" t="s">
         <v>28</v>
       </c>
       <c r="D3" s="2">
@@ -1995,18 +1990,18 @@
       <c r="H3" s="3">
         <v>4131.3013170838403</v>
       </c>
-      <c r="I3" s="6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
+      <c r="I3" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="4" t="s">
         <v>29</v>
       </c>
       <c r="D4" s="2">
@@ -2024,18 +2019,18 @@
       <c r="H4" s="3">
         <v>4025.6378246879299</v>
       </c>
-      <c r="I4" s="6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
+      <c r="I4" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="4" t="s">
         <v>30</v>
       </c>
       <c r="D5" s="2">
@@ -2053,18 +2048,18 @@
       <c r="H5" s="3">
         <v>4427.4478412286899</v>
       </c>
-      <c r="I5" s="6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="6" t="s">
+      <c r="I5" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="4" t="s">
         <v>31</v>
       </c>
       <c r="D6" s="2">
@@ -2082,18 +2077,18 @@
       <c r="H6" s="3">
         <v>2578.24548891733</v>
       </c>
-      <c r="I6" s="6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="6" t="s">
+      <c r="I6" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="4" t="s">
         <v>16</v>
       </c>
       <c r="D7" s="2">
@@ -2111,18 +2106,18 @@
       <c r="H7" s="3">
         <v>1874.7328170251899</v>
       </c>
-      <c r="I7" s="6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
+      <c r="I7" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="4" t="s">
         <v>28</v>
       </c>
       <c r="D8" s="2">
@@ -2140,18 +2135,18 @@
       <c r="H8" s="3">
         <v>946.87732564420503</v>
       </c>
-      <c r="I8" s="6" t="b">
+      <c r="I8" s="4" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="6" t="s">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="4" t="s">
         <v>29</v>
       </c>
       <c r="D9" s="2">
@@ -2169,18 +2164,18 @@
       <c r="H9" s="3">
         <v>3635.5510353936702</v>
       </c>
-      <c r="I9" s="6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
+      <c r="I9" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A10" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="4" t="s">
         <v>30</v>
       </c>
       <c r="D10" s="2">
@@ -2198,18 +2193,18 @@
       <c r="H10" s="3">
         <v>1464.3608375471799</v>
       </c>
-      <c r="I10" s="6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
+      <c r="I10" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A11" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="4" t="s">
         <v>31</v>
       </c>
       <c r="D11" s="2">
@@ -2227,18 +2222,18 @@
       <c r="H11" s="3">
         <v>1021.67721521977</v>
       </c>
-      <c r="I11" s="6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="6" t="s">
+      <c r="I11" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A12" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="4" t="s">
         <v>16</v>
       </c>
       <c r="D12" s="2">
@@ -2256,18 +2251,18 @@
       <c r="H12" s="3">
         <v>780.55260433864703</v>
       </c>
-      <c r="I12" s="6" t="b">
+      <c r="I12" s="4" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="6" t="s">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="4" t="s">
         <v>28</v>
       </c>
       <c r="D13" s="2">
@@ -2285,18 +2280,18 @@
       <c r="H13" s="3">
         <v>1647.0086711199201</v>
       </c>
-      <c r="I13" s="6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="6" t="s">
+      <c r="I13" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A14" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="4" t="s">
         <v>29</v>
       </c>
       <c r="D14" s="2">
@@ -2314,18 +2309,18 @@
       <c r="H14" s="3">
         <v>4344.7811222244</v>
       </c>
-      <c r="I14" s="6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="6" t="s">
+      <c r="I14" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A15" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="4" t="s">
         <v>30</v>
       </c>
       <c r="D15" s="2">
@@ -2343,18 +2338,18 @@
       <c r="H15" s="3">
         <v>3259.3282652063599</v>
       </c>
-      <c r="I15" s="6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="6" t="s">
+      <c r="I15" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A16" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="4" t="s">
         <v>31</v>
       </c>
       <c r="D16" s="2">
@@ -2372,18 +2367,18 @@
       <c r="H16" s="3">
         <v>1309.8784487083999</v>
       </c>
-      <c r="I16" s="6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="6" t="s">
+      <c r="I16" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A17" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="4" t="s">
         <v>16</v>
       </c>
       <c r="D17" s="2">
@@ -2401,18 +2396,18 @@
       <c r="H17" s="3">
         <v>1125.9884671694699</v>
       </c>
-      <c r="I17" s="6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="6" t="s">
+      <c r="I17" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A18" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="4" t="s">
         <v>28</v>
       </c>
       <c r="D18" s="2">
@@ -2430,18 +2425,18 @@
       <c r="H18" s="3">
         <v>2506.5518866866801</v>
       </c>
-      <c r="I18" s="6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="6" t="s">
+      <c r="I18" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A19" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="4" t="s">
         <v>29</v>
       </c>
       <c r="D19" s="2">
@@ -2459,18 +2454,18 @@
       <c r="H19" s="3">
         <v>3108.1095192388998</v>
       </c>
-      <c r="I19" s="6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="6" t="s">
+      <c r="I19" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A20" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="4" t="s">
         <v>30</v>
       </c>
       <c r="D20" s="2">
@@ -2488,18 +2483,18 @@
       <c r="H20" s="3">
         <v>6978.5154644540598</v>
       </c>
-      <c r="I20" s="6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="6" t="s">
+      <c r="I20" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A21" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="C21" s="4" t="s">
         <v>31</v>
       </c>
       <c r="D21" s="2">
@@ -2517,18 +2512,18 @@
       <c r="H21" s="3">
         <v>982.65357634763097</v>
       </c>
-      <c r="I21" s="6" t="b">
+      <c r="I21" s="4" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="6" t="s">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A22" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="C22" s="4" t="s">
         <v>16</v>
       </c>
       <c r="D22" s="2">
@@ -2546,18 +2541,18 @@
       <c r="H22" s="3">
         <v>1216.7294119491501</v>
       </c>
-      <c r="I22" s="6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="6" t="s">
+      <c r="I22" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A23" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="B23" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="C23" s="4" t="s">
         <v>28</v>
       </c>
       <c r="D23" s="2">
@@ -2575,18 +2570,18 @@
       <c r="H23" s="3">
         <v>3122.28346568911</v>
       </c>
-      <c r="I23" s="6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="6" t="s">
+      <c r="I23" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A24" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B24" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="C24" s="4" t="s">
         <v>29</v>
       </c>
       <c r="D24" s="2">
@@ -2604,18 +2599,18 @@
       <c r="H24" s="3">
         <v>3044.9938597803002</v>
       </c>
-      <c r="I24" s="6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="6" t="s">
+      <c r="I24" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A25" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B25" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="C25" s="4" t="s">
         <v>30</v>
       </c>
       <c r="D25" s="2">
@@ -2633,18 +2628,18 @@
       <c r="H25" s="3">
         <v>14824.056900325701</v>
       </c>
-      <c r="I25" s="6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" s="6" t="s">
+      <c r="I25" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A26" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="B26" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="C26" s="4" t="s">
         <v>31</v>
       </c>
       <c r="D26" s="2">
@@ -2662,18 +2657,18 @@
       <c r="H26" s="3">
         <v>1172.35515700114</v>
       </c>
-      <c r="I26" s="6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" s="6" t="s">
+      <c r="I26" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A27" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B27" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="C27" s="4" t="s">
         <v>16</v>
       </c>
       <c r="D27" s="2">
@@ -2691,18 +2686,18 @@
       <c r="H27" s="3">
         <v>2682.4105806992202</v>
       </c>
-      <c r="I27" s="6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A28" s="6" t="s">
+      <c r="I27" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A28" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B28" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C28" s="6" t="s">
+      <c r="C28" s="4" t="s">
         <v>28</v>
       </c>
       <c r="D28" s="2">
@@ -2720,18 +2715,18 @@
       <c r="H28" s="3">
         <v>1427.0232996791201</v>
       </c>
-      <c r="I28" s="6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" s="6" t="s">
+      <c r="I28" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A29" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="B29" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C29" s="6" t="s">
+      <c r="C29" s="4" t="s">
         <v>29</v>
       </c>
       <c r="D29" s="2">
@@ -2749,18 +2744,18 @@
       <c r="H29" s="3">
         <v>1467.65622814424</v>
       </c>
-      <c r="I29" s="6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30" s="6" t="s">
+      <c r="I29" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A30" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="B30" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C30" s="6" t="s">
+      <c r="C30" s="4" t="s">
         <v>30</v>
       </c>
       <c r="D30" s="2">
@@ -2778,18 +2773,18 @@
       <c r="H30" s="3">
         <v>1434.7431889459101</v>
       </c>
-      <c r="I30" s="6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A31" s="6" t="s">
+      <c r="I30" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A31" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="B31" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C31" s="6" t="s">
+      <c r="C31" s="4" t="s">
         <v>31</v>
       </c>
       <c r="D31" s="2">
@@ -2807,18 +2802,18 @@
       <c r="H31" s="3">
         <v>1126.51807543674</v>
       </c>
-      <c r="I31" s="6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" s="6" t="s">
+      <c r="I31" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A32" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B32" s="6" t="s">
+      <c r="B32" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C32" s="6" t="s">
+      <c r="C32" s="4" t="s">
         <v>16</v>
       </c>
       <c r="D32" s="2">
@@ -2836,7 +2831,7 @@
       <c r="H32" s="3">
         <v>929.19610892597495</v>
       </c>
-      <c r="I32" s="6" t="b">
+      <c r="I32" s="4" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2849,23 +2844,23 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:C38"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.81640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.6640625" customWidth="1"/>
-    <col min="9" max="9" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.6328125" customWidth="1"/>
+    <col min="9" max="9" width="15.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D1" s="5" t="s">
         <v>7</v>
       </c>
@@ -2875,7 +2870,7 @@
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -2904,7 +2899,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -2933,7 +2928,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -2962,7 +2957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -2991,7 +2986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -3020,14 +3015,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>1</v>
       </c>
       <c r="B7" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="4" t="s">
         <v>31</v>
       </c>
       <c r="D7" s="2">
@@ -3049,14 +3044,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>1</v>
       </c>
       <c r="B8" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="4" t="s">
         <v>16</v>
       </c>
       <c r="D8" s="2">
@@ -3078,7 +3073,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -3107,7 +3102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -3136,7 +3131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -3165,7 +3160,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -3194,14 +3189,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>2</v>
       </c>
       <c r="B13" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="4" t="s">
         <v>31</v>
       </c>
       <c r="D13" s="2">
@@ -3223,14 +3218,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>2</v>
       </c>
       <c r="B14" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="4" t="s">
         <v>16</v>
       </c>
       <c r="D14" s="2">
@@ -3252,7 +3247,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>3</v>
       </c>
@@ -3281,7 +3276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>3</v>
       </c>
@@ -3310,7 +3305,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>3</v>
       </c>
@@ -3339,7 +3334,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>3</v>
       </c>
@@ -3368,14 +3363,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>3</v>
       </c>
       <c r="B19" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="4" t="s">
         <v>31</v>
       </c>
       <c r="D19" s="2">
@@ -3397,14 +3392,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>3</v>
       </c>
       <c r="B20" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="4" t="s">
         <v>16</v>
       </c>
       <c r="D20" s="2">
@@ -3426,7 +3421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>4</v>
       </c>
@@ -3455,7 +3450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>4</v>
       </c>
@@ -3484,7 +3479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>4</v>
       </c>
@@ -3513,7 +3508,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>4</v>
       </c>
@@ -3542,14 +3537,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>4</v>
       </c>
       <c r="B25" t="s">
         <v>21</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="C25" s="4" t="s">
         <v>31</v>
       </c>
       <c r="D25" s="2">
@@ -3571,14 +3566,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>4</v>
       </c>
       <c r="B26" t="s">
         <v>21</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="C26" s="4" t="s">
         <v>16</v>
       </c>
       <c r="D26" s="2">
@@ -3600,7 +3595,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>5</v>
       </c>
@@ -3629,7 +3624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>5</v>
       </c>
@@ -3658,7 +3653,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>5</v>
       </c>
@@ -3687,7 +3682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>5</v>
       </c>
@@ -3716,14 +3711,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>5</v>
       </c>
       <c r="B31" t="s">
         <v>23</v>
       </c>
-      <c r="C31" s="6" t="s">
+      <c r="C31" s="4" t="s">
         <v>31</v>
       </c>
       <c r="D31" s="2">
@@ -3745,14 +3740,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>5</v>
       </c>
       <c r="B32" t="s">
         <v>23</v>
       </c>
-      <c r="C32" s="6" t="s">
+      <c r="C32" s="4" t="s">
         <v>16</v>
       </c>
       <c r="D32" s="2">
@@ -3774,7 +3769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>6</v>
       </c>
@@ -3803,7 +3798,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>6</v>
       </c>
@@ -3832,7 +3827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>6</v>
       </c>
@@ -3861,7 +3856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>6</v>
       </c>
@@ -3890,14 +3885,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>6</v>
       </c>
       <c r="B37" t="s">
         <v>24</v>
       </c>
-      <c r="C37" s="6" t="s">
+      <c r="C37" s="4" t="s">
         <v>31</v>
       </c>
       <c r="D37" s="2">
@@ -3919,14 +3914,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>6</v>
       </c>
       <c r="B38" t="s">
         <v>24</v>
       </c>
-      <c r="C38" s="6" t="s">
+      <c r="C38" s="4" t="s">
         <v>16</v>
       </c>
       <c r="D38" s="2">
@@ -3957,21 +3952,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.81640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D1" s="5" t="s">
         <v>27</v>
       </c>
@@ -3981,7 +3976,7 @@
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -4010,1047 +4005,1047 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="6" t="s">
         <v>22</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D3">
-        <v>0.218083922856212</v>
-      </c>
-      <c r="E3">
-        <v>0.19725894841480299</v>
-      </c>
-      <c r="F3">
-        <v>0.38033570753233498</v>
-      </c>
-      <c r="G3">
-        <v>1.0067324650046701</v>
-      </c>
-      <c r="H3">
-        <v>318.82479682073898</v>
-      </c>
-      <c r="I3" t="b">
+      <c r="D3" s="7">
+        <v>0.21810582290432701</v>
+      </c>
+      <c r="E3" s="7">
+        <v>0.198335601919995</v>
+      </c>
+      <c r="F3" s="7">
+        <v>0.37676352461090301</v>
+      </c>
+      <c r="G3" s="7">
+        <v>1.00914614361441</v>
+      </c>
+      <c r="H3" s="8">
+        <v>460.33064929734599</v>
+      </c>
+      <c r="I3" s="6" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="6" t="s">
         <v>22</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D4">
-        <v>0.78367156912963798</v>
-      </c>
-      <c r="E4">
-        <v>0.13539596233617399</v>
-      </c>
-      <c r="F4">
-        <v>3.2067390335535499</v>
-      </c>
-      <c r="G4">
-        <v>1.0012349468402599</v>
-      </c>
-      <c r="H4">
-        <v>1847.8424277106501</v>
-      </c>
-      <c r="I4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="D4" s="7">
+        <v>0.85905272995021897</v>
+      </c>
+      <c r="E4" s="7">
+        <v>0.14573758264754599</v>
+      </c>
+      <c r="F4" s="7">
+        <v>3.2414844712989499</v>
+      </c>
+      <c r="G4" s="7">
+        <v>1.00088300653733</v>
+      </c>
+      <c r="H4" s="8">
+        <v>2405.4120383025002</v>
+      </c>
+      <c r="I4" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="6" t="s">
         <v>22</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D5">
-        <v>0.21735397324351899</v>
-      </c>
-      <c r="E5">
-        <v>0.13693316226452401</v>
-      </c>
-      <c r="F5">
-        <v>0.29890801468480099</v>
-      </c>
-      <c r="G5">
-        <v>1.0001188170595201</v>
-      </c>
-      <c r="H5">
-        <v>3529.1529450162998</v>
-      </c>
-      <c r="I5" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="D5" s="7">
+        <v>0.21665260951249901</v>
+      </c>
+      <c r="E5" s="7">
+        <v>0.136584603824698</v>
+      </c>
+      <c r="F5" s="7">
+        <v>0.30162191261864102</v>
+      </c>
+      <c r="G5" s="7">
+        <v>1.00108862679069</v>
+      </c>
+      <c r="H5" s="8">
+        <v>3950.0382140899701</v>
+      </c>
+      <c r="I5" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="6" t="s">
         <v>22</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D6">
-        <v>-2.4059860553939098E-2</v>
-      </c>
-      <c r="E6">
-        <v>-3.32413119478265E-2</v>
-      </c>
-      <c r="F6">
-        <v>-1.4495440611295599E-2</v>
-      </c>
-      <c r="G6">
-        <v>1.00054109216992</v>
-      </c>
-      <c r="H6">
-        <v>2792.1549574024598</v>
-      </c>
-      <c r="I6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="D6" s="7">
+        <v>-2.4097984182683201E-2</v>
+      </c>
+      <c r="E6" s="7">
+        <v>-3.3448193984009701E-2</v>
+      </c>
+      <c r="F6" s="7">
+        <v>-1.4682267323876201E-2</v>
+      </c>
+      <c r="G6" s="7">
+        <v>1.0008153886676501</v>
+      </c>
+      <c r="H6" s="8">
+        <v>3215.9829877751999</v>
+      </c>
+      <c r="I6" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="6" t="s">
         <v>22</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D7">
-        <v>0.34666996558853203</v>
-      </c>
-      <c r="E7">
-        <v>0.30007133596334401</v>
-      </c>
-      <c r="F7">
-        <v>0.39706063821481402</v>
-      </c>
-      <c r="G7">
-        <v>1.00102515995409</v>
-      </c>
-      <c r="H7">
-        <v>2364.9045210119698</v>
-      </c>
-      <c r="I7" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="D7" s="7">
+        <v>0.34627418101434698</v>
+      </c>
+      <c r="E7" s="7">
+        <v>0.299931228261413</v>
+      </c>
+      <c r="F7" s="7">
+        <v>0.39680487924163199</v>
+      </c>
+      <c r="G7" s="7">
+        <v>1.00132652660163</v>
+      </c>
+      <c r="H7" s="8">
+        <v>2252.16432424191</v>
+      </c>
+      <c r="I7" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="6" t="s">
         <v>22</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D8">
-        <v>0.75037963473927805</v>
-      </c>
-      <c r="E8">
-        <v>0.64491975074778396</v>
-      </c>
-      <c r="F8">
-        <v>0.86265160156935194</v>
-      </c>
-      <c r="G8">
-        <v>1.00096595536868</v>
-      </c>
-      <c r="H8">
-        <v>1793.60730278353</v>
-      </c>
-      <c r="I8" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="D8" s="7">
+        <v>0.75082705911133196</v>
+      </c>
+      <c r="E8" s="7">
+        <v>0.64570733568081795</v>
+      </c>
+      <c r="F8" s="7">
+        <v>0.86090514312767796</v>
+      </c>
+      <c r="G8" s="7">
+        <v>1.0014250588097799</v>
+      </c>
+      <c r="H8" s="8">
+        <v>1753.2200269213699</v>
+      </c>
+      <c r="I8" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="6" t="s">
         <v>20</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D9">
-        <v>8.8267680224705894E-2</v>
-      </c>
-      <c r="E9">
-        <v>8.1561175404385497E-2</v>
-      </c>
-      <c r="F9">
-        <v>0.14524812906558701</v>
-      </c>
-      <c r="G9">
-        <v>1.01940888298737</v>
-      </c>
-      <c r="H9">
-        <v>188.36990538293099</v>
-      </c>
-      <c r="I9" t="b">
+      <c r="D9" s="7">
+        <v>8.8030893104585103E-2</v>
+      </c>
+      <c r="E9" s="7">
+        <v>8.16093325254173E-2</v>
+      </c>
+      <c r="F9" s="7">
+        <v>0.12977562774110399</v>
+      </c>
+      <c r="G9" s="7">
+        <v>1.0162714150904399</v>
+      </c>
+      <c r="H9" s="8">
+        <v>434.90733636878201</v>
+      </c>
+      <c r="I9" s="6" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A10" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="6" t="s">
         <v>20</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D10">
-        <v>1.74923089951155</v>
-      </c>
-      <c r="E10">
-        <v>0.42896107196018002</v>
-      </c>
-      <c r="F10">
-        <v>3.4627093804267499</v>
-      </c>
-      <c r="G10">
-        <v>1.0002825622347</v>
-      </c>
-      <c r="H10">
-        <v>4222.4694110742203</v>
-      </c>
-      <c r="I10" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="D10" s="7">
+        <v>1.7561322698286901</v>
+      </c>
+      <c r="E10" s="7">
+        <v>0.47822573347609498</v>
+      </c>
+      <c r="F10" s="7">
+        <v>3.4750430805905701</v>
+      </c>
+      <c r="G10" s="7">
+        <v>1.00010604602002</v>
+      </c>
+      <c r="H10" s="8">
+        <v>4492.1766726235001</v>
+      </c>
+      <c r="I10" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A11" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="6" t="s">
         <v>20</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D11">
-        <v>0.24686145535113399</v>
-      </c>
-      <c r="E11">
-        <v>0.14652834148018101</v>
-      </c>
-      <c r="F11">
-        <v>0.365363048493131</v>
-      </c>
-      <c r="G11">
-        <v>1.0012190043645699</v>
-      </c>
-      <c r="H11">
-        <v>2063.7125810897201</v>
-      </c>
-      <c r="I11" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="D11" s="7">
+        <v>0.25116289236593498</v>
+      </c>
+      <c r="E11" s="7">
+        <v>0.14574042960540201</v>
+      </c>
+      <c r="F11" s="7">
+        <v>0.36444511024405501</v>
+      </c>
+      <c r="G11" s="7">
+        <v>1.0005274731984899</v>
+      </c>
+      <c r="H11" s="8">
+        <v>3367.51223603467</v>
+      </c>
+      <c r="I11" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A12" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="6" t="s">
         <v>20</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D12">
-        <v>-6.77853757346467E-2</v>
-      </c>
-      <c r="E12">
-        <v>-0.104567756798952</v>
-      </c>
-      <c r="F12">
-        <v>-3.5508233115964197E-2</v>
-      </c>
-      <c r="G12">
-        <v>1.0012915040205399</v>
-      </c>
-      <c r="H12">
-        <v>3520.6621068828799</v>
-      </c>
-      <c r="I12" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="D12" s="7">
+        <v>-6.8473365978094697E-2</v>
+      </c>
+      <c r="E12" s="7">
+        <v>-0.104930876492414</v>
+      </c>
+      <c r="F12" s="7">
+        <v>-3.4995770150561899E-2</v>
+      </c>
+      <c r="G12" s="7">
+        <v>0.99981537144744104</v>
+      </c>
+      <c r="H12" s="8">
+        <v>3642.5721122884702</v>
+      </c>
+      <c r="I12" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A13" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="6" t="s">
         <v>20</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D13">
-        <v>0.40620453895534903</v>
-      </c>
-      <c r="E13">
-        <v>0.33768827686355901</v>
-      </c>
-      <c r="F13">
-        <v>0.48586621742084302</v>
-      </c>
-      <c r="G13">
-        <v>1.0023163362507701</v>
-      </c>
-      <c r="H13">
-        <v>1148.9065847776701</v>
-      </c>
-      <c r="I13" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="D13" s="7">
+        <v>0.409057346504622</v>
+      </c>
+      <c r="E13" s="7">
+        <v>0.34100521079888801</v>
+      </c>
+      <c r="F13" s="7">
+        <v>0.48612352093995997</v>
+      </c>
+      <c r="G13" s="7">
+        <v>1.00327800475345</v>
+      </c>
+      <c r="H13" s="8">
+        <v>1357.6973993362701</v>
+      </c>
+      <c r="I13" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A14" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="6" t="s">
         <v>20</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D14">
-        <v>0.30630627998096399</v>
-      </c>
-      <c r="E14">
-        <v>0.25306613250271998</v>
-      </c>
-      <c r="F14">
-        <v>0.36841040578471601</v>
-      </c>
-      <c r="G14">
-        <v>1.00676548172782</v>
-      </c>
-      <c r="H14">
-        <v>675.13948026491698</v>
-      </c>
-      <c r="I14" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="D14" s="7">
+        <v>0.303418876250167</v>
+      </c>
+      <c r="E14" s="7">
+        <v>0.25272124556608999</v>
+      </c>
+      <c r="F14" s="7">
+        <v>0.36179348979442899</v>
+      </c>
+      <c r="G14" s="7">
+        <v>1.0045312499029899</v>
+      </c>
+      <c r="H14" s="8">
+        <v>1146.57074380572</v>
+      </c>
+      <c r="I14" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A15" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="6" t="s">
         <v>19</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D15">
-        <v>0.60455747653916603</v>
-      </c>
-      <c r="E15">
-        <v>0.215133881357989</v>
-      </c>
-      <c r="F15">
-        <v>0.84055885752532999</v>
-      </c>
-      <c r="G15">
-        <v>1.0629534116585</v>
-      </c>
-      <c r="H15">
-        <v>49.152551895762599</v>
-      </c>
-      <c r="I15" t="b">
+      <c r="D15" s="7">
+        <v>0.58577793974312098</v>
+      </c>
+      <c r="E15" s="7">
+        <v>0.21454964057832801</v>
+      </c>
+      <c r="F15" s="7">
+        <v>0.83752455837364004</v>
+      </c>
+      <c r="G15" s="7">
+        <v>1.0292788106801101</v>
+      </c>
+      <c r="H15" s="8">
+        <v>92.579793992742097</v>
+      </c>
+      <c r="I15" s="6" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A16" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="6" t="s">
         <v>19</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D16">
-        <v>1.5648751384633</v>
-      </c>
-      <c r="E16">
-        <v>0.182266448512799</v>
-      </c>
-      <c r="F16">
-        <v>3.5071940944276401</v>
-      </c>
-      <c r="G16">
-        <v>1.0001435519849899</v>
-      </c>
-      <c r="H16">
-        <v>5728.9361429096998</v>
-      </c>
-      <c r="I16" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="D16" s="7">
+        <v>1.58045993193684</v>
+      </c>
+      <c r="E16" s="7">
+        <v>0.17300211067399099</v>
+      </c>
+      <c r="F16" s="7">
+        <v>3.4654612985411299</v>
+      </c>
+      <c r="G16" s="7">
+        <v>1.00126168321042</v>
+      </c>
+      <c r="H16" s="8">
+        <v>6490.7705662397802</v>
+      </c>
+      <c r="I16" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A17" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="6" t="s">
         <v>19</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D17">
-        <v>9.7094734574470806E-2</v>
-      </c>
-      <c r="E17">
-        <v>3.6222763789535303E-2</v>
-      </c>
-      <c r="F17">
-        <v>0.163327004326035</v>
-      </c>
-      <c r="G17">
-        <v>1.0022953650889901</v>
-      </c>
-      <c r="H17">
-        <v>3908.9116485583299</v>
-      </c>
-      <c r="I17" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="D17" s="7">
+        <v>9.7748271792385794E-2</v>
+      </c>
+      <c r="E17" s="7">
+        <v>3.4537433531515602E-2</v>
+      </c>
+      <c r="F17" s="7">
+        <v>0.16352128249328299</v>
+      </c>
+      <c r="G17" s="7">
+        <v>1.00020156625046</v>
+      </c>
+      <c r="H17" s="8">
+        <v>3526.4837689793098</v>
+      </c>
+      <c r="I17" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A18" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="6" t="s">
         <v>19</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D18">
-        <v>-3.5278761042355999E-2</v>
-      </c>
-      <c r="E18">
-        <v>-5.3601911875238203E-2</v>
-      </c>
-      <c r="F18">
-        <v>-1.76170998876298E-2</v>
-      </c>
-      <c r="G18">
-        <v>1.0006110090170499</v>
-      </c>
-      <c r="H18">
-        <v>3935.0237982467402</v>
-      </c>
-      <c r="I18" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="D18" s="7">
+        <v>-3.5235450452438997E-2</v>
+      </c>
+      <c r="E18" s="7">
+        <v>-5.4083944659730099E-2</v>
+      </c>
+      <c r="F18" s="7">
+        <v>-1.7339569307961499E-2</v>
+      </c>
+      <c r="G18" s="7">
+        <v>1.0006665373573</v>
+      </c>
+      <c r="H18" s="8">
+        <v>2877.0177014958099</v>
+      </c>
+      <c r="I18" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A19" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="6" t="s">
         <v>19</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D19">
-        <v>0.36097128012474999</v>
-      </c>
-      <c r="E19">
-        <v>0.31207381082582603</v>
-      </c>
-      <c r="F19">
-        <v>0.41783963031115201</v>
-      </c>
-      <c r="G19">
-        <v>1.00082059689131</v>
-      </c>
-      <c r="H19">
-        <v>1738.61737580209</v>
-      </c>
-      <c r="I19" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+      <c r="D19" s="7">
+        <v>0.36307111717423701</v>
+      </c>
+      <c r="E19" s="7">
+        <v>0.31190708828699498</v>
+      </c>
+      <c r="F19" s="7">
+        <v>0.41772883881700901</v>
+      </c>
+      <c r="G19" s="7">
+        <v>1.0006185912754999</v>
+      </c>
+      <c r="H19" s="8">
+        <v>1719.7088366652799</v>
+      </c>
+      <c r="I19" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A20" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="6" t="s">
         <v>19</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D20">
-        <v>0.25408613549013398</v>
-      </c>
-      <c r="E20">
-        <v>0.20980628242806601</v>
-      </c>
-      <c r="F20">
-        <v>0.30118997588074198</v>
-      </c>
-      <c r="G20">
-        <v>1.00182150996677</v>
-      </c>
-      <c r="H20">
-        <v>996.63806134225399</v>
-      </c>
-      <c r="I20" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+      <c r="D20" s="7">
+        <v>0.25463211201132901</v>
+      </c>
+      <c r="E20" s="7">
+        <v>0.20762293502571499</v>
+      </c>
+      <c r="F20" s="7">
+        <v>0.30604482783571002</v>
+      </c>
+      <c r="G20" s="7">
+        <v>1.0012182958817699</v>
+      </c>
+      <c r="H20" s="8">
+        <v>1020.4823718318401</v>
+      </c>
+      <c r="I20" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A21" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="6" t="s">
         <v>21</v>
       </c>
       <c r="C21" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D21">
-        <v>0.77280776872587498</v>
-      </c>
-      <c r="E21">
-        <v>0.74801554489451505</v>
-      </c>
-      <c r="F21">
-        <v>0.95830473396150295</v>
-      </c>
-      <c r="G21">
-        <v>1.0218166367616699</v>
-      </c>
-      <c r="H21">
-        <v>233.96004780643301</v>
-      </c>
-      <c r="I21" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+      <c r="D21" s="7">
+        <v>0.77374949243007296</v>
+      </c>
+      <c r="E21" s="7">
+        <v>0.75002244734954404</v>
+      </c>
+      <c r="F21" s="7">
+        <v>0.95564775459981999</v>
+      </c>
+      <c r="G21" s="7">
+        <v>1.0008798586957699</v>
+      </c>
+      <c r="H21" s="8">
+        <v>2350.3435494032301</v>
+      </c>
+      <c r="I21" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A22" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="6" t="s">
         <v>21</v>
       </c>
       <c r="C22" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D22">
-        <v>1.0224004009785901</v>
-      </c>
-      <c r="E22">
-        <v>8.4722686287158802E-2</v>
-      </c>
-      <c r="F22">
-        <v>3.0987975553268399</v>
-      </c>
-      <c r="G22">
-        <v>0.99997163660133603</v>
-      </c>
-      <c r="H22">
-        <v>5883.0738781112004</v>
-      </c>
-      <c r="I22" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+      <c r="D22" s="7">
+        <v>1.0229241227146499</v>
+      </c>
+      <c r="E22" s="7">
+        <v>8.3851386571836994E-2</v>
+      </c>
+      <c r="F22" s="7">
+        <v>3.1234490389885998</v>
+      </c>
+      <c r="G22" s="7">
+        <v>1.0007462400856999</v>
+      </c>
+      <c r="H22" s="8">
+        <v>5497.1228080036899</v>
+      </c>
+      <c r="I22" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A23" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="6" t="s">
         <v>21</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D23">
-        <v>6.4306724039302501E-2</v>
-      </c>
-      <c r="E23">
-        <v>2.99415869719502E-2</v>
-      </c>
-      <c r="F23">
-        <v>0.11226763957710501</v>
-      </c>
-      <c r="G23">
-        <v>1.00410327075409</v>
-      </c>
-      <c r="H23">
-        <v>1004.88710238582</v>
-      </c>
-      <c r="I23" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+      <c r="D23" s="7">
+        <v>6.4606539888430098E-2</v>
+      </c>
+      <c r="E23" s="7">
+        <v>2.9467400720645499E-2</v>
+      </c>
+      <c r="F23" s="7">
+        <v>0.119615241072994</v>
+      </c>
+      <c r="G23" s="7">
+        <v>1.0175550426019799</v>
+      </c>
+      <c r="H23" s="8">
+        <v>157.21144487217501</v>
+      </c>
+      <c r="I23" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A24" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="6" t="s">
         <v>21</v>
       </c>
       <c r="C24" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D24">
-        <v>-2.6222519631081499E-2</v>
-      </c>
-      <c r="E24">
-        <v>-4.4012750653735597E-2</v>
-      </c>
-      <c r="F24">
-        <v>-1.2619813074873001E-2</v>
-      </c>
-      <c r="G24">
-        <v>1.00340273584719</v>
-      </c>
-      <c r="H24">
-        <v>963.45791747816702</v>
-      </c>
-      <c r="I24" t="b">
+      <c r="D24" s="7">
+        <v>-2.6326611433933399E-2</v>
+      </c>
+      <c r="E24" s="7">
+        <v>-4.7583480522892997E-2</v>
+      </c>
+      <c r="F24" s="7">
+        <v>-1.28990015670453E-2</v>
+      </c>
+      <c r="G24" s="7">
+        <v>1.0158403247337899</v>
+      </c>
+      <c r="H24" s="8">
+        <v>166.89740053063699</v>
+      </c>
+      <c r="I24" s="6" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A25" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="6" t="s">
         <v>21</v>
       </c>
       <c r="C25" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D25">
-        <v>0.110000539490239</v>
-      </c>
-      <c r="E25">
-        <v>8.3286209728760094E-2</v>
-      </c>
-      <c r="F25">
-        <v>0.15705274485954299</v>
-      </c>
-      <c r="G25">
-        <v>1.00767219824374</v>
-      </c>
-      <c r="H25">
-        <v>400.30159057657301</v>
-      </c>
-      <c r="I25" t="b">
+      <c r="D25" s="7">
+        <v>0.111216263908818</v>
+      </c>
+      <c r="E25" s="7">
+        <v>8.2121766227679693E-2</v>
+      </c>
+      <c r="F25" s="7">
+        <v>0.16874306912499501</v>
+      </c>
+      <c r="G25" s="7">
+        <v>1.02530350971069</v>
+      </c>
+      <c r="H25" s="8">
+        <v>101.246011505588</v>
+      </c>
+      <c r="I25" s="6" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A26" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="6" t="s">
         <v>21</v>
       </c>
       <c r="C26" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D26">
-        <v>0.35072978338093402</v>
-      </c>
-      <c r="E26">
-        <v>0.31665569310157898</v>
-      </c>
-      <c r="F26">
-        <v>0.38391905759174599</v>
-      </c>
-      <c r="G26">
-        <v>1.0009502071965199</v>
-      </c>
-      <c r="H26">
-        <v>1913.5093019855699</v>
-      </c>
-      <c r="I26" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" s="4" t="s">
+      <c r="D26" s="7">
+        <v>0.35042330126509502</v>
+      </c>
+      <c r="E26" s="7">
+        <v>0.30918364393883102</v>
+      </c>
+      <c r="F26" s="7">
+        <v>0.38374934777834802</v>
+      </c>
+      <c r="G26" s="7">
+        <v>1.01850344217047</v>
+      </c>
+      <c r="H26" s="8">
+        <v>171.58095736152799</v>
+      </c>
+      <c r="I26" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A27" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="C27" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D27" s="4">
-        <v>1.00029097738216</v>
-      </c>
-      <c r="E27" s="4">
-        <v>0.63824007412481898</v>
-      </c>
-      <c r="F27" s="4">
-        <v>1.01927407762362</v>
-      </c>
-      <c r="G27" s="4">
-        <v>3.1312241910029499</v>
-      </c>
-      <c r="H27" s="4">
-        <v>2.7083827721542799</v>
-      </c>
-      <c r="I27" s="4" t="b">
+      <c r="D27" s="7">
+        <v>1.0037847770641599</v>
+      </c>
+      <c r="E27" s="7">
+        <v>0.99971066539617903</v>
+      </c>
+      <c r="F27" s="7">
+        <v>1.0254145963286201</v>
+      </c>
+      <c r="G27" s="7">
+        <v>1.00002232482385</v>
+      </c>
+      <c r="H27" s="8">
+        <v>3127.67306569112</v>
+      </c>
+      <c r="I27" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A28" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D28" s="7">
+        <v>1.0899117698528</v>
+      </c>
+      <c r="E28" s="7">
+        <v>0.25944494460148598</v>
+      </c>
+      <c r="F28" s="7">
+        <v>3.0794776290438</v>
+      </c>
+      <c r="G28" s="7">
+        <v>1.0000804357972699</v>
+      </c>
+      <c r="H28" s="8">
+        <v>5755.57975648505</v>
+      </c>
+      <c r="I28" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A29" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D29" s="7">
+        <v>0.15557371365316999</v>
+      </c>
+      <c r="E29" s="7">
+        <v>9.0666660889329204E-2</v>
+      </c>
+      <c r="F29" s="7">
+        <v>0.237985819124236</v>
+      </c>
+      <c r="G29" s="7">
+        <v>1.00318930433918</v>
+      </c>
+      <c r="H29" s="8">
+        <v>1103.0596479344999</v>
+      </c>
+      <c r="I29" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A30" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D30" s="7">
+        <v>-1.08246459887388E-2</v>
+      </c>
+      <c r="E30" s="7">
+        <v>-1.6599632553097699E-2</v>
+      </c>
+      <c r="F30" s="7">
+        <v>-6.3003926551977304E-3</v>
+      </c>
+      <c r="G30" s="7">
+        <v>1.0033004043209399</v>
+      </c>
+      <c r="H30" s="8">
+        <v>1104.2671920483999</v>
+      </c>
+      <c r="I30" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A31" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D31" s="7">
+        <v>8.1764566686227294E-2</v>
+      </c>
+      <c r="E31" s="7">
+        <v>5.9436535558482398E-2</v>
+      </c>
+      <c r="F31" s="7">
+        <v>0.106208199518169</v>
+      </c>
+      <c r="G31" s="7">
+        <v>1.00822500623834</v>
+      </c>
+      <c r="H31" s="8">
+        <v>517.73363592241299</v>
+      </c>
+      <c r="I31" s="6" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A28" s="4" t="s">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A32" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B32" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C28" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D28" s="4">
-        <v>1.62327644363921</v>
-      </c>
-      <c r="E28" s="4">
-        <v>0.28890926010044199</v>
-      </c>
-      <c r="F28" s="4">
-        <v>3.5582875160482499</v>
-      </c>
-      <c r="G28" s="4">
-        <v>1.19092701706826</v>
-      </c>
-      <c r="H28" s="4">
-        <v>7.4300477893872099</v>
-      </c>
-      <c r="I28" s="4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D29" s="4">
-        <v>0.22345662563992</v>
-      </c>
-      <c r="E29" s="4">
-        <v>9.9349700328417404E-2</v>
-      </c>
-      <c r="F29" s="4">
-        <v>1.7352018965132701</v>
-      </c>
-      <c r="G29" s="4">
-        <v>3.4337126547947299</v>
-      </c>
-      <c r="H29" s="4">
-        <v>2.53289063882962</v>
-      </c>
-      <c r="I29" s="4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D30" s="4">
-        <v>-1.55685432925767E-2</v>
-      </c>
-      <c r="E30" s="4">
-        <v>-0.121813169279157</v>
-      </c>
-      <c r="F30" s="4">
-        <v>-6.8744194474760004E-3</v>
-      </c>
-      <c r="G30" s="4">
-        <v>3.3830384575254899</v>
-      </c>
-      <c r="H30" s="4">
-        <v>2.5438425412374799</v>
-      </c>
-      <c r="I30" s="4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A31" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D31" s="4">
-        <v>6.5843382899458694E-2</v>
-      </c>
-      <c r="E31" s="4">
-        <v>9.9661144983280892E-4</v>
-      </c>
-      <c r="F31" s="4">
-        <v>0.10400469423979</v>
-      </c>
-      <c r="G31" s="4">
-        <v>2.6987150122579502</v>
-      </c>
-      <c r="H31" s="4">
-        <v>2.5595836654405799</v>
-      </c>
-      <c r="I31" s="4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C32" s="4" t="s">
+      <c r="C32" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D32" s="4">
-        <v>1.59831588872078</v>
-      </c>
-      <c r="E32" s="4">
-        <v>1.3498580014175701</v>
-      </c>
-      <c r="F32" s="4">
-        <v>2.8019816679204301</v>
-      </c>
-      <c r="G32" s="4">
-        <v>2.8834198110603602</v>
-      </c>
-      <c r="H32" s="4">
-        <v>2.6779957718414602</v>
-      </c>
-      <c r="I32" s="4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
+      <c r="D32" s="7">
+        <v>1.47886758263945</v>
+      </c>
+      <c r="E32" s="7">
+        <v>1.32767204379667</v>
+      </c>
+      <c r="F32" s="7">
+        <v>1.6350279352430701</v>
+      </c>
+      <c r="G32" s="7">
+        <v>1.00239124264235</v>
+      </c>
+      <c r="H32" s="8">
+        <v>1975.5150800915401</v>
+      </c>
+      <c r="I32" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A33" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="6" t="s">
         <v>24</v>
       </c>
       <c r="C33" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D33">
-        <v>0.23396497681348599</v>
-      </c>
-      <c r="E33">
-        <v>6.63779709439698E-2</v>
-      </c>
-      <c r="F33">
-        <v>0.37730376943187299</v>
-      </c>
-      <c r="G33">
-        <v>1.0077963922686899</v>
-      </c>
-      <c r="H33">
-        <v>341.03027568660798</v>
-      </c>
-      <c r="I33" t="b">
+      <c r="D33" s="7">
+        <v>0.22282259711494201</v>
+      </c>
+      <c r="E33" s="7">
+        <v>6.5715574903673996E-2</v>
+      </c>
+      <c r="F33" s="7">
+        <v>0.37293455657816599</v>
+      </c>
+      <c r="G33" s="7">
+        <v>1.0049783491461901</v>
+      </c>
+      <c r="H33" s="8">
+        <v>506.10387077628002</v>
+      </c>
+      <c r="I33" s="6" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A34" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="6" t="s">
         <v>24</v>
       </c>
       <c r="C34" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D34">
-        <v>1.54693386708019</v>
-      </c>
-      <c r="E34">
-        <v>0.27206601306271899</v>
-      </c>
-      <c r="F34">
-        <v>3.4432330004610301</v>
-      </c>
-      <c r="G34">
-        <v>0.99992469638121695</v>
-      </c>
-      <c r="H34">
-        <v>6708.1916769809204</v>
-      </c>
-      <c r="I34" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
+      <c r="D34" s="7">
+        <v>1.54300030564404</v>
+      </c>
+      <c r="E34" s="7">
+        <v>0.27809227963246602</v>
+      </c>
+      <c r="F34" s="7">
+        <v>3.4517461942218302</v>
+      </c>
+      <c r="G34" s="7">
+        <v>1.00052659928404</v>
+      </c>
+      <c r="H34" s="8">
+        <v>5899.1169833207896</v>
+      </c>
+      <c r="I34" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A35" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="6" t="s">
         <v>24</v>
       </c>
       <c r="C35" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D35">
-        <v>6.0611640688942099E-2</v>
-      </c>
-      <c r="E35">
-        <v>1.4259747915306599E-2</v>
-      </c>
-      <c r="F35">
-        <v>0.111766895494465</v>
-      </c>
-      <c r="G35">
-        <v>1.00259860203442</v>
-      </c>
-      <c r="H35">
-        <v>2271.3454448306402</v>
-      </c>
-      <c r="I35" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
+      <c r="D35" s="7">
+        <v>6.1605083312625798E-2</v>
+      </c>
+      <c r="E35" s="7">
+        <v>1.62451537986321E-2</v>
+      </c>
+      <c r="F35" s="7">
+        <v>0.113032796747969</v>
+      </c>
+      <c r="G35" s="7">
+        <v>1.00260455171581</v>
+      </c>
+      <c r="H35" s="8">
+        <v>3155.8392011341398</v>
+      </c>
+      <c r="I35" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A36" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="6" t="s">
         <v>24</v>
       </c>
       <c r="C36" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D36">
-        <v>-1.0785981496093401E-2</v>
-      </c>
-      <c r="E36">
-        <v>-1.9884424113355802E-2</v>
-      </c>
-      <c r="F36">
-        <v>-2.6165786081106201E-3</v>
-      </c>
-      <c r="G36">
-        <v>1.0015589654069199</v>
-      </c>
-      <c r="H36">
-        <v>3060.9723085706801</v>
-      </c>
-      <c r="I36" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
+      <c r="D36" s="7">
+        <v>-1.09460053391481E-2</v>
+      </c>
+      <c r="E36" s="7">
+        <v>-1.96887677129821E-2</v>
+      </c>
+      <c r="F36" s="7">
+        <v>-3.1365025619705801E-3</v>
+      </c>
+      <c r="G36" s="7">
+        <v>1.00209389245167</v>
+      </c>
+      <c r="H36" s="8">
+        <v>3704.8676797165199</v>
+      </c>
+      <c r="I36" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A37" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="6" t="s">
         <v>24</v>
       </c>
       <c r="C37" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D37">
-        <v>0.18418460195317299</v>
-      </c>
-      <c r="E37">
-        <v>0.15043396273544801</v>
-      </c>
-      <c r="F37">
-        <v>0.22242468070436699</v>
-      </c>
-      <c r="G37">
-        <v>1.00338153093282</v>
-      </c>
-      <c r="H37">
-        <v>1356.22972853592</v>
-      </c>
-      <c r="I37" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
+      <c r="D37" s="7">
+        <v>0.184559792584744</v>
+      </c>
+      <c r="E37" s="7">
+        <v>0.151664338149929</v>
+      </c>
+      <c r="F37" s="7">
+        <v>0.22337128073318399</v>
+      </c>
+      <c r="G37" s="7">
+        <v>1.00633286616186</v>
+      </c>
+      <c r="H37" s="8">
+        <v>1133.70183978572</v>
+      </c>
+      <c r="I37" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A38" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="6" t="s">
         <v>24</v>
       </c>
       <c r="C38" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D38">
-        <v>0.57932055959752904</v>
-      </c>
-      <c r="E38">
-        <v>0.48864700664911598</v>
-      </c>
-      <c r="F38">
-        <v>0.681700796772444</v>
-      </c>
-      <c r="G38">
-        <v>1.00428730611963</v>
-      </c>
-      <c r="H38">
-        <v>1425.6119061053</v>
-      </c>
-      <c r="I38" t="b">
+      <c r="D38" s="7">
+        <v>0.57920494553435797</v>
+      </c>
+      <c r="E38" s="7">
+        <v>0.48737996410831302</v>
+      </c>
+      <c r="F38" s="7">
+        <v>0.67763523095606404</v>
+      </c>
+      <c r="G38" s="7">
+        <v>1.00578344313041</v>
+      </c>
+      <c r="H38" s="8">
+        <v>1399.15827961023</v>
+      </c>
+      <c r="I38" s="6" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>